<commit_message>
Markdown updated to calculate perpobility
</commit_message>
<xml_diff>
--- a/data/GlobalRs.xlsx
+++ b/data/GlobalRs.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E580A812-7657-F440-B87A-8BACF7379D4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="10160" yWindow="680" windowWidth="18640" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Citation" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -33,9 +42,6 @@
     <t>Raich (2002)</t>
   </si>
   <si>
-    <t>Peng (2000)</t>
-  </si>
-  <si>
     <t>Year_published</t>
   </si>
   <si>
@@ -63,34 +69,58 @@
     <t>Jian (2018b)</t>
   </si>
   <si>
-    <t>Rh_Reference</t>
-  </si>
-  <si>
     <t>Ra</t>
   </si>
   <si>
-    <t>Ra_Reference</t>
-  </si>
-  <si>
     <t>Rs</t>
   </si>
   <si>
     <t>Rs_Reference</t>
   </si>
   <si>
-    <t>This_study</t>
-  </si>
-  <si>
     <t>Rh</t>
   </si>
   <si>
     <t>CMIP5</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Xu ming (2016)</t>
+  </si>
+  <si>
+    <t>Zhao (2017)</t>
+  </si>
+  <si>
+    <t>环境生态学报</t>
+  </si>
+  <si>
+    <t>陆地生态系统土壤呼吸的观测与模拟</t>
+  </si>
+  <si>
+    <t>Chen (2017)</t>
+  </si>
+  <si>
+    <t>A new estimate of global soil respiration from climate and soil properties</t>
+  </si>
+  <si>
+    <t>Chinese Science Bulletin</t>
+  </si>
+  <si>
+    <t>Cheney (2013)</t>
+  </si>
+  <si>
+    <t>Shimet (1995)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +157,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -135,12 +165,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -182,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +248,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,6 +300,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,52 +492,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="16.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -480,11 +546,11 @@
       <c r="C2" s="1">
         <v>75</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -494,11 +560,11 @@
       <c r="C3" s="1">
         <v>68</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -508,143 +574,156 @@
       <c r="C4" s="1">
         <v>76.5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2000</v>
+        <v>2002</v>
       </c>
       <c r="C5" s="1">
-        <v>69</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <f>80.4</f>
+        <v>80.400000000000006</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2002</v>
+        <v>2010</v>
       </c>
       <c r="C6" s="1">
-        <f>80.4</f>
-        <v>80.400000000000006</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="C7" s="1">
-        <v>98</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="1">
+        <f>15/1.96</f>
+        <v>7.6530612244897958</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C8" s="1">
-        <v>79</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>94.4</v>
+      </c>
+      <c r="D8" s="1">
+        <f>9/1.96</f>
+        <v>4.591836734693878</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="C9" s="1">
-        <v>94.4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="D9" s="1">
+        <f>4/1.96</f>
+        <v>2.0408163265306123</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1">
+        <f>C9-G9</f>
+        <v>50.5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="C10" s="1">
-        <v>91</v>
-      </c>
-      <c r="D10" s="1" t="s">
+        <v>94.3</v>
+      </c>
+      <c r="D10" s="1">
+        <f>17.9/1.96</f>
+        <v>9.1326530612244898</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1">
-        <f>C10-G10</f>
-        <v>50.5</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1">
-        <v>40.5</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C11" s="1">
-        <v>94.3</v>
-      </c>
-      <c r="D11" s="1" t="s">
+        <v>94.5</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="1">
-        <v>59.5</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C12" s="1">
-        <v>94.5</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78.760000000000005</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -652,13 +731,13 @@
         <v>2018</v>
       </c>
       <c r="C13" s="1">
-        <v>78.760000000000005</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88.22</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -666,13 +745,13 @@
         <v>2018</v>
       </c>
       <c r="C14" s="1">
-        <v>76.180000000000007</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70.849999999999994</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -680,13 +759,13 @@
         <v>2018</v>
       </c>
       <c r="C15" s="1">
-        <v>78.34</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66.62</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -694,56 +773,242 @@
         <v>2018</v>
       </c>
       <c r="C16" s="1">
-        <v>72.55</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75.75</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C17" s="1">
-        <v>76.680000000000007</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="1">
-        <v>46.47</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="1">
-        <v>30.21</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71.41</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C18" s="1">
-        <v>71.67</v>
-      </c>
-      <c r="D18" s="1" t="s">
+        <v>80.989999999999995</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C19" s="1">
+        <v>76.180000000000007</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C20" s="1">
+        <v>74.36</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="G18" s="1">
-        <v>25.2</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>20</v>
+      <c r="B21" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C21" s="1">
+        <v>93.29</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C22" s="1">
+        <v>88.58</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C23" s="1">
+        <v>100.72</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C24" s="1">
+        <v>97.01</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C25" s="1">
+        <v>78.34</v>
+      </c>
+      <c r="D25" s="1">
+        <f>4.4/1.96</f>
+        <v>2.2448979591836737</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C26" s="1">
+        <v>72.55</v>
+      </c>
+      <c r="D26" s="1">
+        <f>13.97/1.96</f>
+        <v>7.1275510204081636</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C27" s="1">
+        <v>93.3</v>
+      </c>
+      <c r="D27" s="1">
+        <f>6.1/1.96</f>
+        <v>3.1122448979591835</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="1">
+        <v>59.5</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C28" s="1">
+        <v>120</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -751,25 +1016,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>